<commit_message>
Grobe Use Case Liste
</commit_message>
<xml_diff>
--- a/01_Planung/01_Dokumente/2015_FS_INM21_Requirements_MangelManager.xlsx
+++ b/01_Planung/01_Dokumente/2015_FS_INM21_Requirements_MangelManager.xlsx
@@ -5,23 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HSLU\Java_2\Praxisprojekt\02. Unterlagen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HSLU\Java_2\INM21_Group_B\01_Planung\01_Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="141"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="300" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId1"/>
+    <sheet name="Use Cases" sheetId="4" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="190">
   <si>
     <t xml:space="preserve">Nr. </t>
   </si>
@@ -300,6 +301,297 @@
   </si>
   <si>
     <t>Mängeldaten müssen in Listenform angezeigt und ausgedruckt werden können.</t>
+  </si>
+  <si>
+    <t>Req</t>
+  </si>
+  <si>
+    <t>UseC001</t>
+  </si>
+  <si>
+    <t>UseC002</t>
+  </si>
+  <si>
+    <t>UseC003</t>
+  </si>
+  <si>
+    <t>UseC004</t>
+  </si>
+  <si>
+    <t>UseC005</t>
+  </si>
+  <si>
+    <t>UseC006</t>
+  </si>
+  <si>
+    <t>UseC007</t>
+  </si>
+  <si>
+    <t>UseC008</t>
+  </si>
+  <si>
+    <t>UseC009</t>
+  </si>
+  <si>
+    <t>UseC010</t>
+  </si>
+  <si>
+    <t>UseC011</t>
+  </si>
+  <si>
+    <t>UseC012</t>
+  </si>
+  <si>
+    <t>UseC013</t>
+  </si>
+  <si>
+    <t>UseC014</t>
+  </si>
+  <si>
+    <t>UseC015</t>
+  </si>
+  <si>
+    <t>UseC016</t>
+  </si>
+  <si>
+    <t>UseC017</t>
+  </si>
+  <si>
+    <t>UseC018</t>
+  </si>
+  <si>
+    <t>UseC019</t>
+  </si>
+  <si>
+    <t>UseC020</t>
+  </si>
+  <si>
+    <t>UseC021</t>
+  </si>
+  <si>
+    <t>UseC022</t>
+  </si>
+  <si>
+    <t>UseC023</t>
+  </si>
+  <si>
+    <t>UseC024</t>
+  </si>
+  <si>
+    <t>UseC025</t>
+  </si>
+  <si>
+    <t>UseC026</t>
+  </si>
+  <si>
+    <t>UseC027</t>
+  </si>
+  <si>
+    <t>UseC028</t>
+  </si>
+  <si>
+    <t>UseC029</t>
+  </si>
+  <si>
+    <t>UseC030</t>
+  </si>
+  <si>
+    <t>UseC031</t>
+  </si>
+  <si>
+    <t>UseC032</t>
+  </si>
+  <si>
+    <t>UseC033</t>
+  </si>
+  <si>
+    <t>UseC034</t>
+  </si>
+  <si>
+    <t>UseC035</t>
+  </si>
+  <si>
+    <t>UseC036</t>
+  </si>
+  <si>
+    <t>UseC037</t>
+  </si>
+  <si>
+    <t>UseC038</t>
+  </si>
+  <si>
+    <t>UseC039</t>
+  </si>
+  <si>
+    <t>UseC040</t>
+  </si>
+  <si>
+    <t>Use Case</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Projekt Mängel-Manager - Use Cases</t>
+  </si>
+  <si>
+    <t>SU-Admin erfasst SU-Ansprechperson in SU-Backoffice</t>
+  </si>
+  <si>
+    <t>SU-Admin, SU-Ansprechperson</t>
+  </si>
+  <si>
+    <t>SU-Admin ändert SU-Ansprechperson in SU-Backoffice</t>
+  </si>
+  <si>
+    <t>SU-Admin entfernt SU-Ansprechperson in SU-Backoffice</t>
+  </si>
+  <si>
+    <t>SU-Admin teilt SU-Ansprechperson einem Projekt zu in SU-Backoffice</t>
+  </si>
+  <si>
+    <t>SU-Ansprechperson kann zugeteilte Mängel in SU-UI einsehen</t>
+  </si>
+  <si>
+    <t>SU-Ansprechperson</t>
+  </si>
+  <si>
+    <t>SU-Admin kann Stammdaten modifizieren in SU-Backoffice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SU-Admin </t>
+  </si>
+  <si>
+    <t>SU-Admin</t>
+  </si>
+  <si>
+    <t>SU-Ansprechperson kann Meldung zu Mangel verfassen in SU-UI</t>
+  </si>
+  <si>
+    <t>SU-Ansprechpeson kann Mangel-Kenntnisnahme bestätigen SU-UI</t>
+  </si>
+  <si>
+    <t>SU-Ansprechperson kann Mangel als erledigt markieren in SU-UI</t>
+  </si>
+  <si>
+    <t>SU-Ansprechperson, GU-Bauleiter</t>
+  </si>
+  <si>
+    <t>SU-Admin kann Stammdaten des SU einsehen in SU-Backoffice</t>
+  </si>
+  <si>
+    <t>SU-Ansprechperson kann zugeteilte Projekte einsehen in SU-UI</t>
+  </si>
+  <si>
+    <t>Daten können in UI gefiltert werden</t>
+  </si>
+  <si>
+    <t>Mängelliste aus UI ausdrucken</t>
+  </si>
+  <si>
+    <t>SU Kann Software Online downloaden</t>
+  </si>
+  <si>
+    <t>Req19</t>
+  </si>
+  <si>
+    <t>GU-Admin erfasst Bauherr in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>GU-Admin entfernen Bauherr in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>GU-Admin ändern Bauherr in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>GU-Admin</t>
+  </si>
+  <si>
+    <t>GU-Admin erfasst Bauleiter in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>GU-Admin entfernen Bauleiter in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>GU-Admin ändert Bauleiter in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>GU-Admin erfasst SU in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>GU-Admin entfernt SU in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>GU-Admin ändert SU in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>GU-Admin resettet Passwort für GU-User und SU-Admin</t>
+  </si>
+  <si>
+    <t>GU-Admin erfasst Projekt in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>GU-Admin entfernt Projekt in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>SU-Admin kann alle SU-Projekte einsehen</t>
+  </si>
+  <si>
+    <t>Gu-Admin, GU-Bauleiter</t>
+  </si>
+  <si>
+    <t>GU-Admin, SU</t>
+  </si>
+  <si>
+    <t>GU-Admin, SU-Admin, GU-Bauleiter</t>
+  </si>
+  <si>
+    <t>GU-Admin, GU-Bauleiter</t>
+  </si>
+  <si>
+    <t>GU-Admin ändert ProjektInformationen in GU-Backoffice</t>
+  </si>
+  <si>
+    <t>GU-Bauleiter sieht alle seine Projekte ein in GU-UI</t>
+  </si>
+  <si>
+    <t>GU-Bauleiter erfasst Mangel in GU-UI</t>
+  </si>
+  <si>
+    <t>GU-Bauleiter kann Meldungen einsehen in GU-UI</t>
+  </si>
+  <si>
+    <t>GU-Bauleiter kann Meldungen erfassen in GU-UI</t>
+  </si>
+  <si>
+    <t>UseC041</t>
+  </si>
+  <si>
+    <t>UseC042</t>
+  </si>
+  <si>
+    <t>UseC043</t>
+  </si>
+  <si>
+    <t>UseC044</t>
+  </si>
+  <si>
+    <t>UseC045</t>
+  </si>
+  <si>
+    <t>GU-Bauleiter kann Mangelbehebung bestätigen</t>
+  </si>
+  <si>
+    <t>GU-Bauleiter</t>
+  </si>
+  <si>
+    <t>GU-Bauleiter, SU-Ansprechperson</t>
+  </si>
+  <si>
+    <t>GU-Admin teilt Bauleiter einem Projekt zu</t>
+  </si>
+  <si>
+    <t>User logt sich auf UI ein</t>
   </si>
 </sst>
 </file>
@@ -333,7 +625,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -384,11 +676,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -398,6 +701,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -789,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1293,19 +1604,606 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
-  </headerFooter>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
+    <col min="2" max="2" width="62.453125" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="23" x14ac:dyDescent="0.5">
+      <c r="A1" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1325,4 +2223,22 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>